<commit_message>
vital rates from lit
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurthena\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6015A51E-391F-40CE-A024-11B67AF63582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="2268" windowWidth="17280" windowHeight="8976" firstSheet="5" activeTab="7" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="5070" yWindow="2265" windowWidth="17280" windowHeight="8970" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="NZMS Mortality Rates" sheetId="11" r:id="rId10"/>
     <sheet name="Hydropsyche Mortality Rates" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1037,7 +1036,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1419,16 +1418,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C926AA-9D38-4D93-BFDF-BF59E476DC49}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1436,12 +1435,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>67</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -1457,7 +1456,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>69</v>
       </c>
@@ -1465,7 +1464,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>70</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>71</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>72</v>
       </c>
@@ -1489,7 +1488,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>74</v>
       </c>
@@ -1497,7 +1496,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>73</v>
       </c>
@@ -1505,7 +1504,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>75</v>
       </c>
@@ -1513,12 +1512,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1537,7 +1536,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>167</v>
       </c>
@@ -1545,67 +1544,67 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>196</v>
       </c>
@@ -1616,16 +1615,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667F1D1-AF13-44F8-9E56-B9FD16EB0387}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>317</v>
       </c>
@@ -1667,7 +1666,7 @@
         <v>0.70297029702970293</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -1689,7 +1688,7 @@
         <v>0.70297029702970293</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>0.78712871287128716</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>1.0165016501650166</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -1755,7 +1754,7 @@
         <v>1.0165016501650166</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>223</v>
       </c>
@@ -1783,16 +1782,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA852ABF-0DF7-4B9A-84AF-ADD0D07630EA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -1833,7 +1832,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>302</v>
       </c>
@@ -1854,7 +1853,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>302</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>315</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>0.76747616525423723</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>316</v>
       </c>
@@ -1919,31 +1918,31 @@
         <v>0.76747616525423723</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="2"/>
     </row>
   </sheetData>
@@ -1953,16 +1952,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFC38AF-C57B-434A-A547-824BE01D5EB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -2057,12 +2056,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>214</v>
       </c>
@@ -2076,16 +2075,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{305DC818-8D3E-47F5-BCDD-83A34CDBCF1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2099,7 +2098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>30</v>
       </c>
@@ -2113,7 +2112,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2127,7 +2126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -2141,7 +2140,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>5416.55</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -2224,7 +2223,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>209</v>
       </c>
@@ -2240,16 +2239,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBC5602-3E54-466A-921D-955EC5338DD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>47</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2325,7 +2327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2363,7 +2365,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -2477,7 +2479,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -2515,7 +2517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -2546,7 +2548,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2566,16 +2568,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1CE3E2-B118-495B-9371-003A6BFBB1F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
       <selection activeCell="O213" sqref="O213"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -2598,7 +2600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2621,7 +2623,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -2667,7 +2669,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -2690,7 +2692,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -2713,7 +2715,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>92</v>
       </c>
@@ -2736,7 +2738,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -2759,7 +2761,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2782,7 +2784,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -2802,7 +2804,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -2822,7 +2824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -2862,7 +2864,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2882,8 +2884,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2903,7 +2905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -2920,7 +2922,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>100</v>
       </c>
@@ -2937,7 +2939,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -2954,7 +2956,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2974,7 +2976,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -2994,7 +2996,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3014,7 +3016,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -3034,7 +3036,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -3054,7 +3056,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>103</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -3114,7 +3116,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -3134,7 +3136,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -3154,7 +3156,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -3174,7 +3176,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -3194,7 +3196,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -3214,7 +3216,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -3234,7 +3236,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -3254,7 +3256,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>100</v>
       </c>
@@ -3294,7 +3296,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>103</v>
       </c>
@@ -3314,7 +3316,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -3334,7 +3336,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -3354,7 +3356,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>99</v>
       </c>
@@ -3394,7 +3396,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -3414,7 +3416,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -3434,7 +3436,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -3474,7 +3476,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -3494,7 +3496,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -3514,7 +3516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>107</v>
       </c>
@@ -3534,7 +3536,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>107</v>
       </c>
@@ -3554,7 +3556,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>107</v>
       </c>
@@ -3571,7 +3573,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>127</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>127</v>
       </c>
@@ -3619,7 +3621,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -3636,7 +3638,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -3653,7 +3655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -3670,7 +3672,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3687,7 +3689,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -3704,7 +3706,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3721,7 +3723,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -3738,7 +3740,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3755,7 +3757,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3772,7 +3774,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>146</v>
       </c>
@@ -3789,7 +3791,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>146</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -3823,7 +3825,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>146</v>
       </c>
@@ -3840,7 +3842,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>146</v>
       </c>
@@ -3857,7 +3859,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -3874,7 +3876,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -3891,7 +3893,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>148</v>
       </c>
@@ -3908,7 +3910,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>148</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>148</v>
       </c>
@@ -3942,7 +3944,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>148</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>148</v>
       </c>
@@ -3976,7 +3978,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>148</v>
       </c>
@@ -3993,7 +3995,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>148</v>
       </c>
@@ -4010,7 +4012,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -4027,7 +4029,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>149</v>
       </c>
@@ -4078,7 +4080,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>149</v>
       </c>
@@ -4095,7 +4097,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>149</v>
       </c>
@@ -4112,7 +4114,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>149</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>150</v>
       </c>
@@ -4146,7 +4148,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>150</v>
       </c>
@@ -4163,7 +4165,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>150</v>
       </c>
@@ -4180,7 +4182,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>150</v>
       </c>
@@ -4197,7 +4199,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>150</v>
       </c>
@@ -4214,7 +4216,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>150</v>
       </c>
@@ -4231,7 +4233,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>150</v>
       </c>
@@ -4248,7 +4250,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>147</v>
       </c>
@@ -4265,7 +4267,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>147</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>147</v>
       </c>
@@ -4299,7 +4301,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>147</v>
       </c>
@@ -4316,7 +4318,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>147</v>
       </c>
@@ -4333,7 +4335,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>147</v>
       </c>
@@ -4350,7 +4352,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>147</v>
       </c>
@@ -4374,16 +4376,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B15538-3D4C-42EE-ABFF-D3D33EC7F6D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>218</v>
       </c>
@@ -4415,7 +4417,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>225</v>
       </c>
@@ -4429,7 +4431,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -4443,7 +4445,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -4457,7 +4459,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>240</v>
       </c>
@@ -4474,7 +4476,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -4491,7 +4493,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>244</v>
       </c>
@@ -4508,7 +4510,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>246</v>
       </c>
@@ -4522,7 +4524,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>250</v>
       </c>
@@ -4548,7 +4550,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>253</v>
       </c>
@@ -4574,7 +4576,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>256</v>
       </c>
@@ -4600,7 +4602,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>259</v>
       </c>
@@ -4626,7 +4628,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -4649,7 +4651,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>264</v>
       </c>
@@ -4675,7 +4677,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -4701,7 +4703,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>268</v>
       </c>
@@ -4724,7 +4726,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
         <v>256</v>
       </c>
@@ -4732,7 +4734,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K18" t="s">
         <v>259</v>
       </c>
@@ -4740,7 +4742,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>272</v>
       </c>
@@ -4751,7 +4753,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>271</v>
       </c>
@@ -4762,7 +4764,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>274</v>
       </c>
@@ -4773,7 +4775,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>277</v>
       </c>
@@ -4784,22 +4786,22 @@
         <v>269</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>284</v>
       </c>
@@ -4810,26 +4812,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AA0A0D-C8C4-4B95-9301-D0901FBE12F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -4843,12 +4845,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -4862,7 +4864,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -4873,7 +4875,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>177</v>
       </c>
@@ -4895,7 +4897,7 @@
         <v>2720.5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>179</v>
       </c>
@@ -4909,7 +4911,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>180</v>
       </c>
@@ -4923,7 +4925,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>182</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>183</v>
       </c>
@@ -4951,7 +4953,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -4965,12 +4967,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -4984,12 +4986,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -5001,16 +5003,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7500D613-561D-4AEF-8987-2D25814E2080}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="I73" sqref="I73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -5027,7 +5029,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -5059,7 +5061,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -5082,7 +5084,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -5102,7 +5104,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -5113,7 +5115,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5121,7 +5123,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -5147,7 +5149,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -5171,7 +5173,7 @@
         <v>8.1495383567679967E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>8.1495383567679967E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -5219,7 +5221,7 @@
         <v>4.6180717355018643E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -5243,7 +5245,7 @@
         <v>0.23090358677509323</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -5267,7 +5269,7 @@
         <v>0.70629332425322633</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -5291,7 +5293,7 @@
         <v>6.5196306854143973E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -5323,7 +5325,7 @@
         <v>0.20148148148148148</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -5355,7 +5357,7 @@
         <v>0.20148148148148148</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -5388,7 +5390,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -5420,7 +5422,7 @@
         <v>0.17444444444444443</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>0.17444444444444443</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -5484,7 +5486,7 @@
         <v>0.29437499999999994</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -5516,7 +5518,7 @@
         <v>0.20148148148148148</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -5548,7 +5550,7 @@
         <v>0.20148148148148148</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -5580,7 +5582,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>0.17444444444444443</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>100</v>
       </c>
@@ -5644,7 +5646,7 @@
         <v>0.17444444444444443</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -5676,7 +5678,7 @@
         <v>0.29437499999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>301</v>
       </c>
@@ -5709,7 +5711,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>301</v>
       </c>
@@ -5742,7 +5744,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>301</v>
       </c>
@@ -5775,7 +5777,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -5804,7 +5806,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>302</v>
       </c>
@@ -5833,7 +5835,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>302</v>
       </c>
@@ -5862,7 +5864,7 @@
         <v>1.7755200000113633</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>304</v>
       </c>
@@ -5884,7 +5886,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>304</v>
       </c>
@@ -5906,7 +5908,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>304</v>
       </c>
@@ -5928,7 +5930,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>304</v>
       </c>
@@ -5950,7 +5952,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>304</v>
       </c>
@@ -5972,7 +5974,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>304</v>
       </c>
@@ -5994,7 +5996,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>304</v>
       </c>
@@ -6016,7 +6018,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -6038,7 +6040,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>304</v>
       </c>
@@ -6060,7 +6062,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>304</v>
       </c>
@@ -6082,7 +6084,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>304</v>
       </c>
@@ -6104,7 +6106,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>304</v>
       </c>
@@ -6126,7 +6128,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>304</v>
       </c>
@@ -6148,7 +6150,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>304</v>
       </c>
@@ -6170,7 +6172,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>304</v>
       </c>
@@ -6192,7 +6194,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>304</v>
       </c>
@@ -6214,7 +6216,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>305</v>
       </c>
@@ -6236,7 +6238,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>305</v>
       </c>
@@ -6258,7 +6260,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>305</v>
       </c>
@@ -6280,7 +6282,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>305</v>
       </c>
@@ -6302,7 +6304,7 @@
         <v>0.1867069486404834</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>305</v>
       </c>
@@ -6324,7 +6326,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>305</v>
       </c>
@@ -6346,7 +6348,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>305</v>
       </c>
@@ -6368,7 +6370,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>305</v>
       </c>
@@ -6390,7 +6392,7 @@
         <v>0.1249412554548506</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>305</v>
       </c>
@@ -6412,7 +6414,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>305</v>
       </c>
@@ -6434,7 +6436,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>305</v>
       </c>
@@ -6456,7 +6458,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>305</v>
       </c>
@@ -6478,7 +6480,7 @@
         <v>0.20389392413561599</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>305</v>
       </c>
@@ -6500,7 +6502,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>305</v>
       </c>
@@ -6522,7 +6524,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>305</v>
       </c>
@@ -6544,7 +6546,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>305</v>
       </c>
@@ -6566,7 +6568,7 @@
         <v>5.5052030882846596E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>223</v>
       </c>
@@ -6587,7 +6589,7 @@
         <v>0.49856040682529201</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>223</v>
       </c>
@@ -6604,7 +6606,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>223</v>
       </c>
@@ -6621,7 +6623,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>223</v>
       </c>
@@ -6638,7 +6640,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>140</v>
       </c>
@@ -6660,7 +6662,7 @@
         <v>0.41621621621621613</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>140</v>
       </c>
@@ -6682,7 +6684,7 @@
         <v>2.3486486486486484</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
@@ -6699,11 +6701,11 @@
         <v>0.35</v>
       </c>
       <c r="H71">
-        <f t="shared" ref="H71:H73" si="5">B71/G71</f>
+        <f t="shared" ref="H71:H72" si="5">B71/G71</f>
         <v>0.55714285714285716</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -6724,7 +6726,7 @@
         <v>2.842857142857143</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>310</v>
       </c>
@@ -6746,16 +6748,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A865092E-A2A6-40AC-8BF6-BDD754DDC55D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -6775,7 +6777,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -6800,7 +6802,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>173</v>
       </c>
@@ -6825,7 +6827,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -6850,7 +6852,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -6875,7 +6877,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -6900,7 +6902,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>173</v>
       </c>
@@ -6925,7 +6927,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>173</v>
       </c>
@@ -6950,7 +6952,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>173</v>
       </c>
@@ -6975,7 +6977,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>173</v>
       </c>
@@ -7000,7 +7002,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>173</v>
       </c>
@@ -7025,7 +7027,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Only included Gaufin HYOS temp survival data
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60E5C8D-D29C-44FA-8F8F-EAA38994D436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F6FA95-AF7B-47BD-90C7-F82FBF1FBEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2377" yWindow="3045" windowWidth="17281" windowHeight="9983" firstSheet="9" activeTab="11" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" firstSheet="9" activeTab="11" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="334">
   <si>
     <t>Species</t>
   </si>
@@ -1064,9 +1064,6 @@
   </si>
   <si>
     <t>Gaufin et al., 1972</t>
-  </si>
-  <si>
-    <t>Korboot 1963</t>
   </si>
 </sst>
 </file>
@@ -3707,10 +3704,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5671E9C7-3191-4841-844A-6745CB47FDD2}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3731,13 +3728,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>9.9999999999999995E-8</v>
+        <v>0.99999990000000005</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>18.8</v>
       </c>
       <c r="C2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -3745,7 +3742,7 @@
         <v>0.99999990000000005</v>
       </c>
       <c r="B3">
-        <v>18.8</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C3" t="s">
         <v>333</v>
@@ -3756,7 +3753,7 @@
         <v>0.99999990000000005</v>
       </c>
       <c r="B4">
-        <v>20.399999999999999</v>
+        <v>22.1</v>
       </c>
       <c r="C4" t="s">
         <v>333</v>
@@ -3764,10 +3761,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>0.99999990000000005</v>
+        <v>0.9</v>
       </c>
       <c r="B5">
-        <v>22.1</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>333</v>
@@ -3775,10 +3772,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>333</v>
@@ -3786,10 +3783,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>0.6</v>
+        <v>0.79</v>
       </c>
       <c r="B7">
-        <v>28</v>
+        <v>29.2</v>
       </c>
       <c r="C7" t="s">
         <v>333</v>
@@ -3797,10 +3794,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>0.79</v>
+        <v>0.45</v>
       </c>
       <c r="B8">
-        <v>29.2</v>
+        <v>31.1</v>
       </c>
       <c r="C8" t="s">
         <v>333</v>
@@ -3808,10 +3805,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>0.45</v>
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="B9">
-        <v>31.1</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="C9" t="s">
         <v>333</v>
@@ -3819,23 +3816,12 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>9.9999999999999995E-8</v>
+        <v>1E-8</v>
       </c>
       <c r="B10">
-        <v>32.700000000000003</v>
+        <v>36.5</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>1E-8</v>
-      </c>
-      <c r="B11">
-        <v>36.5</v>
-      </c>
-      <c r="C11" t="s">
         <v>333</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added temp-survival respones from Moffit and James.
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F6FA95-AF7B-47BD-90C7-F82FBF1FBEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6556AD2-9C5D-46A5-9595-D60AEC89D95D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" firstSheet="9" activeTab="11" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="5700" yWindow="3697" windowWidth="17280" windowHeight="9983" firstSheet="13" activeTab="13" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="334">
   <si>
     <t>Species</t>
   </si>
@@ -1051,9 +1051,6 @@
     <t>Cox &amp; Rutherford, 2000</t>
   </si>
   <si>
-    <t>Zaranko et al., 1997</t>
-  </si>
-  <si>
     <t>MaturationRate</t>
   </si>
   <si>
@@ -1064,6 +1061,9 @@
   </si>
   <si>
     <t>Gaufin et al., 1972</t>
+  </si>
+  <si>
+    <t>Moffit &amp; James, 2012</t>
   </si>
 </sst>
 </file>
@@ -3706,8 +3706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5671E9C7-3191-4841-844A-6745CB47FDD2}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3734,7 +3734,7 @@
         <v>18.8</v>
       </c>
       <c r="C2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -3745,7 +3745,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="C3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -3756,7 +3756,7 @@
         <v>22.1</v>
       </c>
       <c r="C4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -3767,7 +3767,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -3778,7 +3778,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -3789,7 +3789,7 @@
         <v>29.2</v>
       </c>
       <c r="C7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -3800,7 +3800,7 @@
         <v>31.1</v>
       </c>
       <c r="C8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -3811,7 +3811,7 @@
         <v>32.700000000000003</v>
       </c>
       <c r="C9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -3822,7 +3822,7 @@
         <v>36.5</v>
       </c>
       <c r="C10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3968,10 +3968,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4A60B5-2702-4A70-9CB2-3B17A88B6CEB}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4039,7 +4039,29 @@
         <v>1E-4</v>
       </c>
       <c r="C6" t="s">
-        <v>329</v>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -7379,7 +7401,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B1" t="s">
         <v>325</v>
@@ -7396,7 +7418,7 @@
         <v>6.9</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -7407,7 +7429,7 @@
         <v>7.66</v>
       </c>
       <c r="C3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -7418,7 +7440,7 @@
         <v>8.67</v>
       </c>
       <c r="C4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -7429,7 +7451,7 @@
         <v>12.1</v>
       </c>
       <c r="C5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -7440,7 +7462,7 @@
         <v>2.86</v>
       </c>
       <c r="C6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -7451,7 +7473,7 @@
         <v>3.28</v>
       </c>
       <c r="C7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -7462,7 +7484,7 @@
         <v>1.35</v>
       </c>
       <c r="C8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -7473,7 +7495,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="C9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -7484,7 +7506,7 @@
         <v>34.4</v>
       </c>
       <c r="C10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Chironomidae vital rates
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60E5C8D-D29C-44FA-8F8F-EAA38994D436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA90181D-3FAF-43F0-A08C-85D0A40785F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2377" yWindow="3045" windowWidth="17281" windowHeight="9983" firstSheet="9" activeTab="11" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="3885" yWindow="6180" windowWidth="17280" windowHeight="9982" firstSheet="15" activeTab="17" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -25,10 +25,12 @@
     <sheet name="Mortality Rates" sheetId="6" r:id="rId10"/>
     <sheet name="Baetid Mortality Rates" sheetId="10" r:id="rId11"/>
     <sheet name="Hydropsyche Survival Rates " sheetId="16" r:id="rId12"/>
-    <sheet name="Baetid Survival Rates" sheetId="12" r:id="rId13"/>
-    <sheet name="NZMS Survival Rates" sheetId="14" r:id="rId14"/>
-    <sheet name="NZMS Mortality Rates" sheetId="11" r:id="rId15"/>
-    <sheet name="Hydropsyche Mortality Rates" sheetId="9" r:id="rId16"/>
+    <sheet name="Chiro Survival" sheetId="17" r:id="rId13"/>
+    <sheet name="Baetid Survival Rates" sheetId="12" r:id="rId14"/>
+    <sheet name="NZMS Survival Rates" sheetId="14" r:id="rId15"/>
+    <sheet name="NZMS Mortality Rates" sheetId="11" r:id="rId16"/>
+    <sheet name="Hydropsyche Mortality Rates" sheetId="9" r:id="rId17"/>
+    <sheet name="Sheet4" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="339">
   <si>
     <t>Species</t>
   </si>
@@ -1067,6 +1069,18 @@
   </si>
   <si>
     <t>Korboot 1963</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Eggermont &amp; Heiri, 2012</t>
+  </si>
+  <si>
+    <t>Max/Bankful</t>
+  </si>
+  <si>
+    <t>(no mortality - increase)</t>
   </si>
 </sst>
 </file>
@@ -1159,9 +1173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1199,7 +1213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1305,7 +1319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1447,7 +1461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1654,8 +1668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7500D613-561D-4AEF-8987-2D25814E2080}">
   <dimension ref="A1:N73"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="G85" sqref="G85"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3400,7 +3414,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3709,7 +3723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5671E9C7-3191-4841-844A-6745CB47FDD2}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3845,6 +3859,120 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C77117-34E9-45B5-AFFE-43A5629D5643}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>16.43762508</v>
+      </c>
+      <c r="C2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>44.807415470000002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>0.30897791499999999</v>
+      </c>
+      <c r="C5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>69.146448509999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>84.645904290000004</v>
+      </c>
+      <c r="C7" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>54.50651311</v>
+      </c>
+      <c r="C8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>9.5137108949999991</v>
+      </c>
+      <c r="C9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648851F1-1B76-483B-BD38-93D8FC0F4DDF}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -3980,7 +4108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F4A60B5-2702-4A70-9CB2-3B17A88B6CEB}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -4061,7 +4189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667F1D1-AF13-44F8-9E56-B9FD16EB0387}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4228,12 +4356,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA852ABF-0DF7-4B9A-84AF-ADD0D07630EA}">
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4395,6 +4523,257 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826C251F-8D33-462C-AE02-50288781B133}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>0.3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2">
+        <v>36.8119011</v>
+      </c>
+      <c r="G2">
+        <f>B2/F2</f>
+        <v>8.1495383567679967E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>1.7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3">
+        <v>36.8119011</v>
+      </c>
+      <c r="G3">
+        <f>B3/F3</f>
+        <v>4.6180717355018643E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>8.5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4">
+        <v>36.8119011</v>
+      </c>
+      <c r="G4">
+        <f>B4/F4</f>
+        <v>0.23090358677509323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F5">
+        <v>36.8119011</v>
+      </c>
+      <c r="G5">
+        <f>B5/F5</f>
+        <v>0.70629332425322633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.747</v>
+      </c>
+      <c r="D6" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6">
+        <v>2.7</v>
+      </c>
+      <c r="G6">
+        <f>B6/F6</f>
+        <v>0.20148148148148148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F7">
+        <v>2.7</v>
+      </c>
+      <c r="G7">
+        <f>B7/F7</f>
+        <v>0.20148148148148148</v>
+      </c>
+      <c r="H7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>1.6</v>
+      </c>
+      <c r="G8">
+        <f>B8/F8</f>
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="D9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F9">
+        <v>2.7</v>
+      </c>
+      <c r="G9">
+        <f>B9/F9</f>
+        <v>0.17444444444444443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>300</v>
+      </c>
+      <c r="F10">
+        <v>2.7</v>
+      </c>
+      <c r="G10">
+        <f>B10/F10</f>
+        <v>0.17444444444444443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>300</v>
+      </c>
+      <c r="F11">
+        <v>1.6</v>
+      </c>
+      <c r="G11">
+        <f>B11/F11</f>
+        <v>0.29437499999999994</v>
+      </c>
+      <c r="H11" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5141,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1CE3E2-B118-495B-9371-003A6BFBB1F7}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="O213" sqref="O213"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7510,7 +7889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AA0A0D-C8C4-4B95-9301-D0901FBE12F4}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added sheet with growth rate data for NZMS
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5416E6C4-E881-416C-A68C-B59438385DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B4F52E-9148-4BB4-A7DD-E5620197BD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="17279" windowHeight="9982" firstSheet="11" activeTab="11" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="1770" yWindow="2453" windowWidth="17280" windowHeight="9982" firstSheet="16" activeTab="18" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="NZMS Mortality Rates" sheetId="11" r:id="rId16"/>
     <sheet name="Hydropsyche Mortality Rates" sheetId="9" r:id="rId17"/>
     <sheet name="Chiro Mortality Rates" sheetId="18" r:id="rId18"/>
+    <sheet name="Sheet3" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="353">
   <si>
     <t>Species</t>
   </si>
@@ -1114,6 +1115,15 @@
   </si>
   <si>
     <t>Stratment et al. 2014</t>
+  </si>
+  <si>
+    <t>NZMS Growth Rate (mm/mo)</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>Dybdahl &amp; Kane, 2005</t>
   </si>
 </sst>
 </file>
@@ -3772,7 +3782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5671E9C7-3191-4841-844A-6745CB47FDD2}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -5434,6 +5444,131 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D5572D-33FE-4713-A31D-A4A12D21A4AC}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="C2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="C3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="C4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1.28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>1.29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>1.74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFC38AF-C57B-434A-A547-824BE01D5EB3}">
   <dimension ref="A1:L12"/>

</xml_diff>

<commit_message>
vital rates with G. lacustris data
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E51E0F-2175-4E2F-81D1-3DE5E39DE3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8B2BC0-09CD-47ED-B976-4BFE123F7111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="17280" windowHeight="10522" firstSheet="20" activeTab="21" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="17280" windowHeight="10522" firstSheet="20" activeTab="22" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,8 @@
     <sheet name="Chiro Mortality Rates" sheetId="18" r:id="rId20"/>
     <sheet name="Sheet3" sheetId="19" r:id="rId21"/>
     <sheet name="Gammarus Survival Rates" sheetId="20" r:id="rId22"/>
-    <sheet name="Gammarus Mortality Rates" sheetId="22" r:id="rId23"/>
+    <sheet name="Sheet7" sheetId="25" r:id="rId23"/>
+    <sheet name="Gammarus Mortality Rates" sheetId="22" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6128,7 +6129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BAB039-2530-4577-9F3B-6EE9D5C56715}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -6465,6 +6466,20 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3036D474-192E-46E4-BAEA-4B877C888235}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA253E9-1F1C-44C1-9CF5-B4F18C2F916B}">
   <dimension ref="A1:R24"/>
   <sheetViews>

</xml_diff>

<commit_message>
deleted cross ref in NZMS
</commit_message>
<xml_diff>
--- a/VitalRates.xlsx
+++ b/VitalRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jelly\Documents\ColoradoRiverInverts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DD39D2-DFF3-4B76-B651-12BD0D1B8F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E876BDAF-1D9D-446B-8149-858A0C31B084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="14595" firstSheet="14" activeTab="15" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="17280" windowHeight="10523" firstSheet="17" activeTab="18" xr2:uid="{5BBB9DFD-573C-4E7C-88D7-10047BA5B2E6}"/>
   </bookViews>
   <sheets>
     <sheet name="To Read" sheetId="4" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="370">
   <si>
     <t>Species</t>
   </si>
@@ -4442,7 +4442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C77117-34E9-45B5-AFFE-43A5629D5643}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
@@ -5190,15 +5190,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8667F1D1-AF13-44F8-9E56-B9FD16EB0387}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>317</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>0.70297029702970293</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>317</v>
       </c>
@@ -5262,7 +5262,7 @@
         <v>0.70297029702970293</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>317</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>0.78712871287128716</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>1.0165016501650166</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -5326,27 +5326,6 @@
       <c r="F6">
         <f t="shared" si="0"/>
         <v>1.0165016501650166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="K7" t="s">
-        <v>317</v>
-      </c>
-      <c r="L7">
-        <v>1200</v>
-      </c>
-      <c r="M7">
-        <v>0.6855</v>
-      </c>
-      <c r="N7" t="s">
-        <v>307</v>
-      </c>
-      <c r="O7">
-        <v>2406.9299999999998</v>
-      </c>
-      <c r="P7">
-        <f>L7/O7</f>
-        <v>0.49856040682529201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>